<commit_message>
Kisi-kisi export to excel
</commit_message>
<xml_diff>
--- a/public/excel_template/Kisi_Kisi_Template.xlsx
+++ b/public/excel_template/Kisi_Kisi_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\API-Login-Register\public\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47258B4C-1D32-47B0-996A-BFB312CB69A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB385A3-909D-44E9-9BDC-87446564FAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,9 +28,6 @@
     <t>SUMATIF AKHIR SEMESTER ( SAS ) GENAP</t>
   </si>
   <si>
-    <t>TAHUN PELAJARAN 2022/2023</t>
-  </si>
-  <si>
     <t>ALOKASI WAKTU</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>PILIHAN GANDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAHUN PELAJARAN </t>
   </si>
 </sst>
 </file>
@@ -283,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -320,22 +320,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -344,10 +353,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,7 +576,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C13" sqref="C13:F13"/>
@@ -578,18 +587,18 @@
     <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -597,11 +606,11 @@
     <row r="2" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -609,11 +618,11 @@
     <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="34"/>
+      <c r="E3" s="24"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -643,27 +652,27 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="1"/>
       <c r="E7" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="23"/>
       <c r="I7" s="1"/>
@@ -671,29 +680,29 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="1"/>
       <c r="E8" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="16"/>
       <c r="I9" s="1"/>
@@ -731,15 +740,15 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="34"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -747,12 +756,12 @@
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="29"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -760,12 +769,12 @@
     <row r="15" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -773,15 +782,15 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="20" t="s">
         <v>13</v>
-      </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="20" t="s">
-        <v>14</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -790,100 +799,24 @@
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
       <c r="B17" s="21"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="26"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="22"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="22"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="22"/>
-    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="8">
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C3:E3"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove title from excel
</commit_message>
<xml_diff>
--- a/public/excel_template/Kisi_Kisi_Template.xlsx
+++ b/public/excel_template/Kisi_Kisi_Template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\API-Login-Register\public\excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB385A3-909D-44E9-9BDC-87446564FAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA503EE1-3B55-48AF-8AD7-76CB0C18A054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kisi-Kisi Soal SAS Genap Matema" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheets1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -578,8 +578,8 @@
   </sheetPr>
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>